<commit_message>
Added updated xslx test spreadsheet and adjusted value assertions to match contents.
</commit_message>
<xml_diff>
--- a/io-xlsx/src/test/resources/test1.xlsx
+++ b/io-xlsx/src/test/resources/test1.xlsx
@@ -376,7 +376,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,7 +423,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>12.2</v>
+        <v>12.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>